<commit_message>
Challenge initialisation and test in main
</commit_message>
<xml_diff>
--- a/Challenges.xlsx
+++ b/Challenges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonarddesportes/Desktop/Projet-WebApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CFD1332-1EEF-A547-B5F5-7C1CB0C1B970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE5B3F-8200-EE4A-9AFC-D059336D347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1260" windowWidth="28040" windowHeight="16880" xr2:uid="{6E18BB8E-CF48-F745-85C6-F0D4DB86BC04}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{6E18BB8E-CF48-F745-85C6-F0D4DB86BC04}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Defi</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>soriety_score</t>
+  </si>
+  <si>
+    <t>Defi ton voisin de droite au pierre feuille ciseau, celui qui pert bois 3 gorgées</t>
   </si>
 </sst>
 </file>
@@ -110,16 +113,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,18 +435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DE189E-3724-F647-9BA1-CE15407DBF8A}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -459,7 +459,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -473,7 +473,21 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>